<commit_message>
Updates in data followers
</commit_message>
<xml_diff>
--- a/CollectNationality Distribution.xlsx
+++ b/CollectNationality Distribution.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="92">
   <si>
     <t>NASA</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>Pierre</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -660,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1184,7 +1187,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -1192,7 +1195,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -1200,7 +1203,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>5</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>10</v>
       </c>
@@ -1224,7 +1227,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>13</v>
       </c>
@@ -1232,7 +1235,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>18</v>
       </c>
@@ -1240,7 +1243,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>21</v>
       </c>
@@ -1248,7 +1251,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>26</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>29</v>
       </c>
@@ -1264,7 +1267,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>34</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>37</v>
       </c>
@@ -1280,7 +1283,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -1288,7 +1291,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>45</v>
       </c>
@@ -1296,7 +1299,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>50</v>
       </c>
@@ -1304,76 +1307,103 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>53</v>
       </c>
       <c r="B80" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>58</v>
       </c>
       <c r="B81" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>61</v>
       </c>
       <c r="B82" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>66</v>
       </c>
       <c r="B83" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="C83" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>69</v>
       </c>
       <c r="B84" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>74</v>
       </c>
       <c r="B85" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="C85" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>77</v>
       </c>
       <c r="B86" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="C86" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>82</v>
       </c>
       <c r="B87" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="C87" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>85</v>
       </c>
       <c r="B88" t="s">
         <v>90</v>
+      </c>
+      <c r="C88" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data collection Pierre followers location
</commit_message>
<xml_diff>
--- a/CollectNationality Distribution.xlsx
+++ b/CollectNationality Distribution.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="92">
   <si>
     <t>NASA</t>
   </si>
@@ -666,7 +666,7 @@
   <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1274,6 +1274,9 @@
       <c r="B75" t="s">
         <v>90</v>
       </c>
+      <c r="C75" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
@@ -1282,6 +1285,9 @@
       <c r="B76" t="s">
         <v>90</v>
       </c>
+      <c r="C76" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
@@ -1290,6 +1296,9 @@
       <c r="B77" t="s">
         <v>90</v>
       </c>
+      <c r="C77" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
@@ -1297,6 +1306,9 @@
       </c>
       <c r="B78" t="s">
         <v>90</v>
+      </c>
+      <c r="C78" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:3">

</xml_diff>

<commit_message>
Update Pierre Data Collection
</commit_message>
<xml_diff>
--- a/CollectNationality Distribution.xlsx
+++ b/CollectNationality Distribution.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="16000" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="92">
   <si>
     <t>NASA</t>
   </si>
@@ -666,7 +666,7 @@
   <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1250,6 +1250,9 @@
       <c r="B72" t="s">
         <v>90</v>
       </c>
+      <c r="C72" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
@@ -1258,6 +1261,9 @@
       <c r="B73" t="s">
         <v>90</v>
       </c>
+      <c r="C73" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
@@ -1265,6 +1271,9 @@
       </c>
       <c r="B74" t="s">
         <v>90</v>
+      </c>
+      <c r="C74" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:3">

</xml_diff>

<commit_message>
kelly changes made 3/24≈
</commit_message>
<xml_diff>
--- a/CollectNationality Distribution.xlsx
+++ b/CollectNationality Distribution.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="1580" yWindow="0" windowWidth="12100" windowHeight="16320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="92">
   <si>
     <t>NASA</t>
   </si>
@@ -301,10 +301,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -327,13 +350,178 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="83">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -665,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -675,303 +863,412 @@
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
       <c r="B13" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
       <c r="B14" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>40</v>
       </c>
       <c r="B16" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
       <c r="B17" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
       <c r="B18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
       <c r="B19" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>51</v>
       </c>
       <c r="B20" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>54</v>
       </c>
       <c r="B21" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>56</v>
       </c>
       <c r="B22" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>59</v>
       </c>
       <c r="B23" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>62</v>
       </c>
       <c r="B24" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>64</v>
       </c>
       <c r="B25" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>67</v>
       </c>
       <c r="B26" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>70</v>
       </c>
       <c r="B27" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>72</v>
       </c>
       <c r="B28" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>75</v>
       </c>
       <c r="B29" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>78</v>
       </c>
       <c r="B30" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>80</v>
       </c>
       <c r="B31" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>83</v>
       </c>
       <c r="B32" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>86</v>
       </c>
       <c r="B33" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>1</v>
       </c>
       <c r="B34" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>4</v>
       </c>
       <c r="B35" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>7</v>
       </c>
       <c r="B36" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>9</v>
       </c>
       <c r="B37" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -979,15 +1276,18 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>15</v>
       </c>
       <c r="B39" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -995,7 +1295,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>20</v>
       </c>
@@ -1003,7 +1303,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -1011,7 +1311,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -1019,7 +1319,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>28</v>
       </c>
@@ -1027,7 +1327,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -1035,7 +1335,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -1043,7 +1343,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -1051,7 +1351,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -1059,7 +1359,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -1067,7 +1367,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>44</v>
       </c>
@@ -1075,116 +1375,158 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>47</v>
       </c>
       <c r="B51" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
       <c r="B52" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>55</v>
       </c>
       <c r="B54" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>57</v>
       </c>
       <c r="B55" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>60</v>
       </c>
       <c r="B56" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>63</v>
       </c>
       <c r="B57" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>65</v>
       </c>
       <c r="B58" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
       <c r="B59" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>71</v>
       </c>
       <c r="B60" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>73</v>
       </c>
       <c r="B61" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>76</v>
       </c>
       <c r="B62" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>79</v>
       </c>
       <c r="B63" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>81</v>
       </c>
       <c r="B64" t="s">
         <v>89</v>
+      </c>
+      <c r="C64" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1194,6 +1536,9 @@
       <c r="B65" t="s">
         <v>89</v>
       </c>
+      <c r="C65" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
@@ -1202,6 +1547,9 @@
       <c r="B66" t="s">
         <v>89</v>
       </c>
+      <c r="C66" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
@@ -1226,6 +1574,9 @@
       <c r="B69" t="s">
         <v>90</v>
       </c>
+      <c r="C69" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
@@ -1234,6 +1585,9 @@
       <c r="B70" t="s">
         <v>90</v>
       </c>
+      <c r="C70" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
@@ -1241,6 +1595,9 @@
       </c>
       <c r="B71" t="s">
         <v>90</v>
+      </c>
+      <c r="C71" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1435,6 +1792,7 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>